<commit_message>
[mod] update 2019-08-23 19:40
</commit_message>
<xml_diff>
--- a/CAH.xlsx
+++ b/CAH.xlsx
@@ -10,10 +10,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="5">
+  <numFmts count="3">
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="177" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="390" formatCode="yyyy-MM-dd"/>
     <numFmt numFmtId="391" formatCode="yyyy-MM-dd\ HH:mm:ss"/>
   </numFmts>
@@ -398,31 +396,31 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B2" t="str">
-        <v>请勿将_放入_</v>
+        <v>如果在课堂上_的话学校生活就结束了</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B3" t="str">
-        <v>__虽好，但不要贪杯</v>
+        <v>卡面来打</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B4" t="str">
-        <v>你们先走！我__</v>
+        <v>岛摄</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B5" t="str">
-        <v>警方在现场找到一具高度损坏的男性遗体，死因经检测为_</v>
+        <v>roll点</v>
       </c>
     </row>
     <row r="6">
@@ -430,7 +428,7 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B6" t="str">
-        <v>人不能，至少不应该_</v>
+        <v>只有_才能_</v>
       </c>
     </row>
     <row r="7">
@@ -438,15 +436,15 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B7" t="str">
-        <v>一开口就知道，老_了</v>
+        <v>我一_发现_在_</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B8" t="str">
-        <v>无内鬼，来点_笑话</v>
+        <v>撸管</v>
       </c>
     </row>
     <row r="9">
@@ -454,7 +452,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B9" t="str">
-        <v>隔壁超市薯片半价</v>
+        <v>看小马</v>
       </c>
     </row>
     <row r="10">
@@ -462,15 +460,15 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B10" t="str">
-        <v>光头</v>
+        <v>阴阳</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B11" t="str">
-        <v>随着“咔嚓”一声脆响，从蛋里钻出来一只_</v>
+        <v>肥父</v>
       </c>
     </row>
     <row r="12">
@@ -478,7 +476,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B12" t="str">
-        <v>美洲大蠊</v>
+        <v>丧尸</v>
       </c>
     </row>
     <row r="13">
@@ -486,7 +484,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B13" t="str">
-        <v>蟑螂</v>
+        <v>肥肥</v>
       </c>
     </row>
     <row r="14">
@@ -494,7 +492,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B14" t="str">
-        <v>擦过精液的卫生纸</v>
+        <v>沙包</v>
       </c>
     </row>
     <row r="15">
@@ -502,7 +500,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B15" t="str">
-        <v>新鲜出炉的华莱士</v>
+        <v>角虫</v>
       </c>
     </row>
     <row r="16">
@@ -510,15 +508,15 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B16" t="str">
-        <v>炸鸡，西瓜，葡萄汽水</v>
+        <v>一般通过肥肥</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B17" t="str">
-        <v>我最喜欢的食物是_</v>
+        <v>飞蛾的排泄物</v>
       </c>
     </row>
     <row r="18">
@@ -526,15 +524,15 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B18" t="str">
-        <v>人民广场1080度狂拽炫酷吊炸天大回旋空中手冲连续技</v>
+        <v>小碎骨</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B19" t="str">
-        <v>我最喜欢_</v>
+        <v>匿名版偶像</v>
       </c>
     </row>
     <row r="20">
@@ -542,7 +540,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B20" t="str">
-        <v>抽烟喝酒烫头</v>
+        <v>uk酱</v>
       </c>
     </row>
     <row r="21">
@@ -550,7 +548,7 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B21" t="str">
-        <v>这里禁止养_</v>
+        <v>_我草泥马</v>
       </c>
     </row>
     <row r="22">
@@ -558,7 +556,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B22" t="str">
-        <v>穆斯林</v>
+        <v>资本主义</v>
       </c>
     </row>
     <row r="23">
@@ -566,7 +564,7 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B23" t="str">
-        <v>我_今天就是要一拳打爆你_的狗头</v>
+        <v>天下漫友是一家,_</v>
       </c>
     </row>
     <row r="24">
@@ -574,15 +572,15 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B24" t="str">
-        <v>阳光大姐</v>
+        <v>bog生来没有ma</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B25" t="str">
-        <v>喵喵酱</v>
+        <v>您的_没了</v>
       </c>
     </row>
     <row r="26">
@@ -590,7 +588,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B26" t="str">
-        <v>狗比酱</v>
+        <v>马</v>
       </c>
     </row>
     <row r="27">
@@ -598,7 +596,7 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B27" t="str">
-        <v>请问您今天要来点_吗？</v>
+        <v>_是_,而且是_的_你喜欢吗？</v>
       </c>
     </row>
     <row r="28">
@@ -606,31 +604,31 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B28" t="str">
-        <v>路过的假面骑士</v>
+        <v>r20</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B29" t="str">
-        <v>名侦探_</v>
+        <v>前列腺</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B30" t="str">
-        <v>-我喜欢用_做施法时的配菜。 -淦，老兄，你的性癖好jb怪啊！</v>
+        <v>女装</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B31" t="str">
-        <v>我要成为新世界的_</v>
+        <v>射精管理</v>
       </c>
     </row>
     <row r="32">
@@ -638,7 +636,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B32" t="str">
-        <v>AC娘</v>
+        <v>NTR</v>
       </c>
     </row>
     <row r="33">
@@ -646,39 +644,39 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B33" t="str">
-        <v>黄脸婆</v>
+        <v>看本子</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B34" t="str">
-        <v>快手同款_，火热销售中！</v>
+        <v>撸管</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B35" t="str">
-        <v>特朗普最新表态：_</v>
+        <v>喷射</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B36" t="str">
-        <v>这就是国家一级保护动物，_</v>
+        <v>吃华莱士</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B37" t="str">
-        <v>_即是正义！</v>
+        <v>刘姥姥</v>
       </c>
     </row>
     <row r="38">
@@ -686,7 +684,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B38" t="str">
-        <v>巨乳</v>
+        <v>斯大林</v>
       </c>
     </row>
     <row r="39">
@@ -694,7 +692,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B39" t="str">
-        <v>贫乳</v>
+        <v>喇叭</v>
       </c>
     </row>
     <row r="40">
@@ -702,7 +700,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B40" t="str">
-        <v>辣椒酱抹菊花</v>
+        <v>黄金体验镇魂曲</v>
       </c>
     </row>
     <row r="41">
@@ -710,15 +708,15 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B41" t="str">
-        <v>用大蒜汁泡屌</v>
+        <v>白金之星</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B42" t="str">
-        <v>_超骚</v>
+        <v>疯狂钻石</v>
       </c>
     </row>
     <row r="43">
@@ -726,7 +724,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B43" t="str">
-        <v>牙签搅大缸</v>
+        <v>砸瓦鲁多</v>
       </c>
     </row>
     <row r="44">
@@ -734,7 +732,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B44" t="str">
-        <v>可口可乐</v>
+        <v>绯红之王</v>
       </c>
     </row>
     <row r="45">
@@ -742,7 +740,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B45" t="str">
-        <v>百事可乐</v>
+        <v>杀手皇后</v>
       </c>
     </row>
     <row r="46">
@@ -750,15 +748,15 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B46" t="str">
-        <v>甜豆腐脑天下第一</v>
+        <v>天堂制造</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B47" t="str">
-        <v>咸豆腐脑天下第一</v>
+        <v>_3000</v>
       </c>
     </row>
     <row r="48">
@@ -766,15 +764,15 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B48" t="str">
-        <v>有基佬开我裤链</v>
+        <v>黄金回旋</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B49" t="str">
-        <v>禁止在厕所_</v>
+        <v>芦苇娘</v>
       </c>
     </row>
     <row r="50">
@@ -782,7 +780,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B50" t="str">
-        <v>2333gkd那是真的批爆</v>
+        <v>阿苇</v>
       </c>
     </row>
     <row r="51">
@@ -790,15 +788,15 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B51" t="str">
-        <v>雪菜碧池</v>
+        <v>vtuber</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B52" t="str">
-        <v>冬马小三</v>
+        <v>忘了他吧，我_养你</v>
       </c>
     </row>
     <row r="53">
@@ -806,7 +804,7 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B53" t="str">
-        <v>-天呐，比尔！你在干什么？你怎么能杀人！ -_     -你这比青蛙小便还下流的家伙，就由我的猎枪制裁。</v>
+        <v>真鸡儿_</v>
       </c>
     </row>
     <row r="54">
@@ -814,15 +812,15 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B54" t="str">
-        <v>批里批里淦杯</v>
+        <v>金属</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B55" t="str">
-        <v>学学比尔</v>
+        <v>_也就图一乐，真想还得_</v>
       </c>
     </row>
     <row r="56">
@@ -830,7 +828,7 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B56" t="str">
-        <v>_才有怜悯之心，我没有</v>
+        <v>全新抖音同款ins风潮流时尚生日礼物居家必备多功能万用懒人网红爆款特惠限量版_</v>
       </c>
     </row>
     <row r="57">
@@ -838,23 +836,23 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B57" t="str">
-        <v>对不起，我是_</v>
+        <v>任天堂是世界的_，索尼是宇宙的_!</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B58" t="str">
-        <v>以前我没得选择，现在我想做个_</v>
+        <v>全世界的独立游戏制作人</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B59" t="str">
-        <v>这是失传已久的_神功！你到底是谁！</v>
+        <v>努力做到尿尿不分叉</v>
       </c>
     </row>
     <row r="60">
@@ -862,7 +860,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B60" t="str">
-        <v>被杀</v>
+        <v>傻逼一号卢本伟准备就绪</v>
       </c>
     </row>
     <row r="61">
@@ -870,15 +868,15 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B61" t="str">
-        <v>人_，就会死。</v>
+        <v>在bilibili突然发现了_</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B62" t="str">
-        <v>没有什么比爱情的力量更强大，除了_</v>
+        <v>手冲</v>
       </c>
     </row>
     <row r="63">
@@ -886,23 +884,23 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B63" t="str">
-        <v>空中转体两周半</v>
+        <v>远在委内瑞拉的独立游戏制作人</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B64" t="str">
-        <v>_，你一定不懂吧。</v>
+        <v>叙利亚打工仔</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B65" t="str">
-        <v>_现已加入肯德基豪华午餐</v>
+        <v>new了一个对象</v>
       </c>
     </row>
     <row r="66">
@@ -910,31 +908,31 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B66" t="str">
-        <v>他居然使用_挡下了所有的攻击！</v>
+        <v>尊敬的客户，您的_已到期，请及时充值</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B67" t="str">
-        <v>在变身魔法少女之后裸奔，结果被城管抓走</v>
+        <v>寻找_特别行动小组，近日宣称_。</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B68" t="str">
-        <v>只有我一个人_吗？</v>
+        <v>胶佬</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B69" t="str">
-        <v>五分钟带你看完_</v>
+        <v>手游玩家</v>
       </c>
     </row>
     <row r="70">
@@ -942,7 +940,7 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B70" t="str">
-        <v>《_名言选》是今年的畅销书</v>
+        <v>因为群员发布了_视频，群主被公开_。</v>
       </c>
     </row>
     <row r="71">
@@ -950,7 +948,7 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B71" t="str">
-        <v>你在嫖娼时发现，这里的头牌居然是_</v>
+        <v>steam就是_启动器！</v>
       </c>
     </row>
     <row r="72">
@@ -958,7 +956,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B72" t="str">
-        <v>穿着女装的你爸</v>
+        <v>恰柠檬</v>
       </c>
     </row>
     <row r="73">
@@ -966,7 +964,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B73" t="str">
-        <v>青梅竹马</v>
+        <v>反人类卡牌</v>
       </c>
     </row>
     <row r="74">
@@ -974,15 +972,15 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B74" t="str">
-        <v>你爸的跳蛋漏电了</v>
+        <v>小黄油</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B75" t="str">
-        <v>_批发，量大从优</v>
+        <v>空气模拟器</v>
       </c>
     </row>
     <row r="76">
@@ -990,7 +988,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B76" t="str">
-        <v>看幼女视频</v>
+        <v>进入了坦克</v>
       </c>
     </row>
     <row r="77">
@@ -998,7 +996,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B77" t="str">
-        <v>幼男</v>
+        <v>成为了微博红人榜最耀眼的星</v>
       </c>
     </row>
     <row r="78">
@@ -1006,7 +1004,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B78" t="str">
-        <v>幼女</v>
+        <v>单推孙笑川</v>
       </c>
     </row>
     <row r="79">
@@ -1014,15 +1012,15 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B79" t="str">
-        <v>在厕所日马桶排水口</v>
+        <v>暗杀刘波</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B80" t="str">
-        <v>用套套吹气球</v>
+        <v>我要成为_偶像，说罢裁判便抛下了妻女离去了。</v>
       </c>
     </row>
     <row r="81">
@@ -1030,7 +1028,7 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B81" t="str">
-        <v>你被捕了，因为你_</v>
+        <v>听众朋友们欢迎收听深夜_广播节目，我是你们的好朋友_。</v>
       </c>
     </row>
     <row r="82">
@@ -1038,7 +1036,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B82" t="str">
-        <v>兽耳娘</v>
+        <v>裁判</v>
       </c>
     </row>
     <row r="83">
@@ -1046,7 +1044,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B83" t="str">
-        <v>furry</v>
+        <v>最后回答者</v>
       </c>
     </row>
     <row r="84">
@@ -1054,7 +1052,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B84" t="str">
-        <v>尼哥</v>
+        <v>获胜者</v>
       </c>
     </row>
     <row r="85">
@@ -1062,7 +1060,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B85" t="str">
-        <v>(　^ω^)</v>
+        <v>打开了斗鱼7078973</v>
       </c>
     </row>
     <row r="86">
@@ -1070,7 +1068,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B86" t="str">
-        <v>(ノﾟ∀ﾟ)ノ举高高</v>
+        <v>用舌头走路</v>
       </c>
     </row>
     <row r="87">
@@ -1078,7 +1076,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B87" t="str">
-        <v>城墙</v>
+        <v>在抗日剧中参演日本天皇</v>
       </c>
     </row>
     <row r="88">
@@ -1086,15 +1084,15 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B88" t="str">
-        <v>哇(=ﾟωﾟ)=</v>
+        <v>乔碧萝殿下</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B89" t="str">
-        <v>这就是_吗？</v>
+        <v>郭德纲</v>
       </c>
     </row>
     <row r="90">
@@ -1102,7 +1100,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B90" t="str">
-        <v>切尔诺贝利</v>
+        <v>于谦</v>
       </c>
     </row>
     <row r="91">
@@ -1110,15 +1108,15 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B91" t="str">
-        <v>马眼</v>
+        <v>女装少年</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B92" t="str">
-        <v>恨不得把蛋都塞进_里</v>
+        <v>大龄异装癖</v>
       </c>
     </row>
     <row r="93">
@@ -1126,7 +1124,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B93" t="str">
-        <v>里神乐</v>
+        <v>ATM</v>
       </c>
     </row>
     <row r="94">
@@ -1134,15 +1132,15 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B94" t="str">
-        <v>真tm牛逼，搞得我想一拳打进_的_里。</v>
+        <v>为什么你会_！，难道你是_！？</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B95" t="str">
-        <v>做超屌的720度大回旋</v>
+        <v>_一度成为2019年朝鲜最最流行。</v>
       </c>
     </row>
     <row r="96">
@@ -1150,7 +1148,7 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B96" t="str">
-        <v>我们可以看到，监控画面中的这位男子正在_</v>
+        <v>众所周知反人类卡牌除了白卡和黑卡，还有_卡。</v>
       </c>
     </row>
     <row r="97">
@@ -1158,7 +1156,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B97" t="str">
-        <v>妹妹的内裤</v>
+        <v>你妈升天</v>
       </c>
     </row>
     <row r="98">
@@ -1166,15 +1164,15 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B98" t="str">
-        <v>上上下下左左右右BABA</v>
+        <v>大香肠</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B99" t="str">
-        <v>活塞运动</v>
+        <v>_说：“是你守护了我吗？_”</v>
       </c>
     </row>
     <row r="100">
@@ -1182,39 +1180,39 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B100" t="str">
-        <v>狂拽炫酷吊炸天</v>
+        <v>国产3A神作</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B101" t="str">
-        <v>发色图</v>
+        <v>_爱上了_，在一个有星星的夜晚</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B102" t="str">
-        <v>台妹</v>
+        <v>经证实，被_撞飞至40米高空的_，被判为碰瓷行为，现已依法入狱。</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B103" t="str">
-        <v>N98</v>
+        <v>为了攻打养老院我们派出了，20多名英勇的_。</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B104" t="str">
-        <v>微积分</v>
+        <v>《恋上妹妹的_》一经发售便风靡全球</v>
       </c>
     </row>
     <row r="105">
@@ -1222,31 +1220,31 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B105" t="str">
-        <v>-今天岛上没有智障 -淦！是_！</v>
+        <v>公司新增一个_岗位，月薪近20W。</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B106" t="str">
-        <v>你们没有_吗？</v>
+        <v>逼乎大神</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B107" t="str">
-        <v>这个版本我们决定削弱_，增强_</v>
+        <v>啊</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B108" t="str">
-        <v>宝藏男孩</v>
+        <v>看_也就图一乐，真要_还得看_</v>
       </c>
     </row>
     <row r="109">
@@ -1254,7 +1252,7 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B109" t="str">
-        <v>这是是什么神仙_啊！</v>
+        <v>看到这个我气得浑身发抖， 大热天的全身冷汗，手脚冰凉， 这个社会还能不能好了， 到底要怎么样你们才满意 眼泪不争气的流了下来 ，_上到处充斥着对 _的压迫， 他们何时才能真正的站起来？</v>
       </c>
     </row>
     <row r="110">
@@ -1262,31 +1260,31 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B110" t="str">
-        <v>-我就是憨批之王   -_ _    -你赢了</v>
+        <v>无内鬼，发点_</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B111" t="str">
-        <v>欧拉欧拉欧拉</v>
+        <v>重生之我是_</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B112" t="str">
-        <v>欧吉车技腐乳句句然到雾入饭卡死了</v>
+        <v>我_ ，在那儿他们都叫我_ ！</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B113" t="str">
-        <v>滚铁环</v>
+        <v>说起来很下流，我看见_boki了</v>
       </c>
     </row>
     <row r="114">
@@ -1294,55 +1292,55 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B114" t="str">
-        <v>-施主，这是什么漫画？ -是_</v>
+        <v>我支持_ ！你们可以打我了！</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B115" t="str">
-        <v>jojo</v>
+        <v>_，FBI Open up！</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B116" t="str">
-        <v>自私的神</v>
+        <v>人不能_，至少不该</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B117" t="str">
-        <v>施主</v>
+        <v>天哪！这是什么神仙_鸭！！我坐地排卵！</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B118" t="str">
-        <v>三个月没洗的</v>
+        <v>在_有一个永恒话题，那就是_</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B119" t="str">
-        <v>草莓幼女</v>
+        <v>《如果早知道_也会被性侵》</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B120" t="str">
-        <v>草莓糖浆</v>
+        <v>都9012年了，你还在_？</v>
       </c>
     </row>
     <row r="121">
@@ -1350,7 +1348,7 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B121" t="str">
-        <v>人群中钻出来一个_</v>
+        <v>_2077</v>
       </c>
     </row>
     <row r="122">
@@ -1358,7 +1356,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B122" t="str">
-        <v>机械烈海王</v>
+        <v>海绵宝宝</v>
       </c>
     </row>
     <row r="123">
@@ -1366,7 +1364,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B123" t="str">
-        <v>你妈炸了</v>
+        <v>感染菜花</v>
       </c>
     </row>
     <row r="124">
@@ -1374,7 +1372,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B124" t="str">
-        <v>塞进菊花</v>
+        <v>出卖斯大林</v>
       </c>
     </row>
     <row r="125">
@@ -1382,7 +1380,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B125" t="str">
-        <v>徐逸</v>
+        <v>跑团</v>
       </c>
     </row>
     <row r="126">
@@ -1390,23 +1388,23 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B126" t="str">
-        <v>陈睿</v>
+        <v>魔法少女</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B127" t="str">
-        <v>没有_便无法_了吗？，_岂是如此不便之物！</v>
+        <v>键盘侠</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B128" t="str">
-        <v>百般武艺，此乃_</v>
+        <v>野兽先辈</v>
       </c>
     </row>
     <row r="129">
@@ -1414,39 +1412,39 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B129" t="str">
-        <v>飞天大草</v>
+        <v>倒悬打飞机</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B130" t="str">
-        <v>鲨鱼抱枕</v>
+        <v>那么答案只有一个了！_ _</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B131" t="str">
-        <v>洛阳亲友如相问，_ _</v>
+        <v>向你宣誓效忠</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B132" t="str">
-        <v>向你宣誓效忠</v>
+        <v>洛阳亲友如相问，_ _</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B133" t="str">
-        <v>那么答案只有一个了！_ _</v>
+        <v>鲨鱼抱枕</v>
       </c>
     </row>
     <row r="134">
@@ -1454,23 +1452,23 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B134" t="str">
-        <v>倒悬打飞机</v>
+        <v>飞天大草</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B135" t="str">
-        <v>野兽先辈</v>
+        <v>百般武艺，此乃_</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B136" t="str">
-        <v>键盘侠</v>
+        <v>没有_便无法_了吗？，_岂是如此不便之物！</v>
       </c>
     </row>
     <row r="137">
@@ -1478,7 +1476,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B137" t="str">
-        <v>魔法少女</v>
+        <v>陈睿</v>
       </c>
     </row>
     <row r="138">
@@ -1486,7 +1484,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B138" t="str">
-        <v>d20</v>
+        <v>徐逸</v>
       </c>
     </row>
     <row r="139">
@@ -1494,7 +1492,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B139" t="str">
-        <v>跑团</v>
+        <v>塞进菊花</v>
       </c>
     </row>
     <row r="140">
@@ -1502,7 +1500,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B140" t="str">
-        <v>出卖斯大林</v>
+        <v>你妈炸了</v>
       </c>
     </row>
     <row r="141">
@@ -1510,63 +1508,63 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B141" t="str">
-        <v>感染菜花</v>
+        <v>机械烈海王</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B142" t="str">
-        <v>海绵宝宝</v>
+        <v>人群中钻出来一个_</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B143" t="str">
-        <v>_2077</v>
+        <v>草莓糖浆</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B144" t="str">
-        <v>都9012年了，你还在_？</v>
+        <v>草莓幼女</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B145" t="str">
-        <v>《如果早知道_也会被性侵》</v>
+        <v>三个月没洗的</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B146" t="str">
-        <v>在_有一个永恒话题，那就是_</v>
+        <v>施主</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B147" t="str">
-        <v>天哪！这是什么神仙_鸭！！我坐地排卵！</v>
+        <v>自私的神</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B148" t="str">
-        <v>人不能_，至少不该</v>
+        <v>jojo</v>
       </c>
     </row>
     <row r="149">
@@ -1574,31 +1572,31 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B149" t="str">
-        <v>_，FBI Open up！</v>
+        <v>-施主，这是什么漫画？ -是_</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B150" t="str">
-        <v>我支持_ ！你们可以打我了！</v>
+        <v>滚铁环</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B151" t="str">
-        <v>说起来很下流，我看见_boki了</v>
+        <v>欧吉车技腐乳句句然到雾入饭卡死了</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B152" t="str">
-        <v>我_ ，在那儿他们都叫我_ ！</v>
+        <v>欧拉欧拉欧拉</v>
       </c>
     </row>
     <row r="153">
@@ -1606,7 +1604,7 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B153" t="str">
-        <v>重生之我是_</v>
+        <v>-我就是憨批之王   -__    -你赢了</v>
       </c>
     </row>
     <row r="154">
@@ -1614,15 +1612,15 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B154" t="str">
-        <v>无内鬼，发点_</v>
+        <v>这是是什么神仙_啊！</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B155" t="str">
-        <v>看到这个我气得浑身发抖， 大热天的全身冷汗，手脚冰凉， 这个社会还能不能好了， 到底要怎么样你们才满意 眼泪不争气的流了下来 ，_上到处充斥着对 _的压迫， 他们何时才能真正的站起来？</v>
+        <v>宝藏男孩</v>
       </c>
     </row>
     <row r="156">
@@ -1630,31 +1628,31 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B156" t="str">
-        <v>看_也就图一乐，真要_还得看_</v>
+        <v>这个版本我们决定削弱_，增强_</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B157" t="str">
-        <v>啊</v>
+        <v>你们没有_吗？</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B158" t="str">
-        <v>逼乎大神</v>
+        <v>-今天岛上没有智障 -淦！是_！</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B159" t="str">
-        <v>公司新增一个_岗位，月薪近20W。</v>
+        <v>微积分</v>
       </c>
     </row>
     <row r="160">
@@ -1662,31 +1660,31 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B160" t="str">
-        <v>《恋上妹妹的_》一经发售便风靡全球</v>
+        <v>N98</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B161" t="str">
-        <v>为了攻打养老院我们派出了，20多名英勇的_。</v>
+        <v>台妹</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B162" t="str">
-        <v>经证实，被_撞飞至40米高空的_，被判为碰瓷行为，现已依法入狱。</v>
+        <v>发色图</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B163" t="str">
-        <v>_爱上了_，在一个有星星的夜晚</v>
+        <v>狂拽炫酷吊炸天</v>
       </c>
     </row>
     <row r="164">
@@ -1694,15 +1692,15 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B164" t="str">
-        <v>国产3A神作</v>
+        <v>活塞运动</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B165" t="str">
-        <v>_说：“是你守护了我吗？_”</v>
+        <v>上上下下左左右右BABA</v>
       </c>
     </row>
     <row r="166">
@@ -1710,15 +1708,15 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B166" t="str">
-        <v>都难以分离......</v>
+        <v>妹妹的内裤</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B167" t="str">
-        <v>大香肠</v>
+        <v>我们可以看到，监控画面中的这位男子正在_</v>
       </c>
     </row>
     <row r="168">
@@ -1726,7 +1724,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B168" t="str">
-        <v>你妈升天</v>
+        <v>做超屌的720度大回旋</v>
       </c>
     </row>
     <row r="169">
@@ -1734,15 +1732,15 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B169" t="str">
-        <v>众所周知反人类卡牌除了白卡和黑卡，还有_卡。</v>
+        <v>真tm牛逼，搞得我想一拳打进_的_里。</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B170" t="str">
-        <v>_一度成为2019年朝鲜最最流行。</v>
+        <v>里神乐</v>
       </c>
     </row>
     <row r="171">
@@ -1750,7 +1748,7 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B171" t="str">
-        <v>为什么你会_！，难道你是_！？</v>
+        <v>恨不得把蛋都塞进_里</v>
       </c>
     </row>
     <row r="172">
@@ -1758,7 +1756,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B172" t="str">
-        <v>ATM</v>
+        <v>马眼</v>
       </c>
     </row>
     <row r="173">
@@ -1766,15 +1764,15 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B173" t="str">
-        <v>大龄异装癖</v>
+        <v>切尔诺贝利</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B174" t="str">
-        <v>女装少年</v>
+        <v>这就是_吗？</v>
       </c>
     </row>
     <row r="175">
@@ -1782,7 +1780,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B175" t="str">
-        <v>于谦</v>
+        <v>哇(=ﾟωﾟ)=</v>
       </c>
     </row>
     <row r="176">
@@ -1790,7 +1788,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B176" t="str">
-        <v>郭德纲</v>
+        <v>城墙</v>
       </c>
     </row>
     <row r="177">
@@ -1798,7 +1796,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B177" t="str">
-        <v>乔碧萝殿下</v>
+        <v>(ノﾟ∀ﾟ)ノ举高高</v>
       </c>
     </row>
     <row r="178">
@@ -1806,7 +1804,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B178" t="str">
-        <v>在抗日剧中参演日本天皇</v>
+        <v>(　^ω^)</v>
       </c>
     </row>
     <row r="179">
@@ -1814,7 +1812,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B179" t="str">
-        <v>用舌头走路</v>
+        <v>尼哥</v>
       </c>
     </row>
     <row r="180">
@@ -1822,7 +1820,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B180" t="str">
-        <v>打开了斗鱼7078973</v>
+        <v>furry</v>
       </c>
     </row>
     <row r="181">
@@ -1830,15 +1828,15 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B181" t="str">
-        <v>获胜者</v>
+        <v>兽耳娘</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B182" t="str">
-        <v>最后回答者</v>
+        <v>你被捕了，因为你_</v>
       </c>
     </row>
     <row r="183">
@@ -1846,23 +1844,23 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B183" t="str">
-        <v>裁判</v>
+        <v>用套套吹气球</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B184" t="str">
-        <v>听众朋友们欢迎收听深夜_广播节目，我是你们的好朋友_。</v>
+        <v>在厕所日马桶排水口</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B185" t="str">
-        <v>我要成为_偶像，说罢裁判便抛下了妻女离去了。</v>
+        <v>幼女</v>
       </c>
     </row>
     <row r="186">
@@ -1870,7 +1868,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B186" t="str">
-        <v>暗杀刘波</v>
+        <v>幼男</v>
       </c>
     </row>
     <row r="187">
@@ -1878,15 +1876,15 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B187" t="str">
-        <v>单推孙笑川</v>
+        <v>看幼女视频</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B188" t="str">
-        <v>成为了微博红人榜最耀眼的星</v>
+        <v>_批发，量大从优</v>
       </c>
     </row>
     <row r="189">
@@ -1894,7 +1892,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B189" t="str">
-        <v>进入了坦克</v>
+        <v>你爸的跳蛋漏电了</v>
       </c>
     </row>
     <row r="190">
@@ -1902,7 +1900,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B190" t="str">
-        <v>空气模拟器</v>
+        <v>青梅竹马</v>
       </c>
     </row>
     <row r="191">
@@ -1910,23 +1908,23 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B191" t="str">
-        <v>小黄油</v>
+        <v>穿着女装的你爸</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B192" t="str">
-        <v>反人类卡牌</v>
+        <v>你在嫖娼时发现，这里的头牌居然是_</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B193" t="str">
-        <v>恰柠檬</v>
+        <v>《_名言选》是今年的畅销书</v>
       </c>
     </row>
     <row r="194">
@@ -1934,7 +1932,7 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B194" t="str">
-        <v>steam就是_启动器！</v>
+        <v>五分钟带你看完_</v>
       </c>
     </row>
     <row r="195">
@@ -1942,7 +1940,7 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B195" t="str">
-        <v>因为群员发布了_视频，群主被公开_。</v>
+        <v>只有我一个人_吗？</v>
       </c>
     </row>
     <row r="196">
@@ -1950,23 +1948,23 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B196" t="str">
-        <v>手游玩家</v>
+        <v>在变身魔法少女之后裸奔，结果被城管抓走</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B197" t="str">
-        <v>胶佬</v>
+        <v>他居然使用_挡下了所有的攻击！</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B198" t="str">
-        <v>寻找_特别行动小组，近日宣称_。</v>
+        <v>_现已加入肯德基豪华午餐</v>
       </c>
     </row>
     <row r="199">
@@ -1974,7 +1972,7 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B199" t="str">
-        <v>尊敬的客户，您的_已到期，请及时充值</v>
+        <v>_，你一定不懂吧。</v>
       </c>
     </row>
     <row r="200">
@@ -1982,23 +1980,23 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B200" t="str">
-        <v>new了一个对象</v>
+        <v>空中转体两周半</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B201" t="str">
-        <v>叙利亚打工仔</v>
+        <v>没有什么比爱情的力量更强大，除了_</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B202" t="str">
-        <v>远在委内瑞拉的独立游戏制作人</v>
+        <v>人_，就会死。</v>
       </c>
     </row>
     <row r="203">
@@ -2006,7 +2004,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B203" t="str">
-        <v>手冲</v>
+        <v>被杀</v>
       </c>
     </row>
     <row r="204">
@@ -2014,47 +2012,47 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B204" t="str">
-        <v>在bilibili突然发现了_</v>
+        <v>这是失传已久的_神功！你到底是谁！</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B205" t="str">
-        <v>傻逼一号卢本伟准备就绪</v>
+        <v>以前我没得选择，现在我想做个_</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B206" t="str">
-        <v>努力做到尿尿不分叉</v>
+        <v>对不起，我是_</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B207" t="str">
-        <v>全世界的独立游戏制作人</v>
+        <v>_才有怜悯之心，我没有</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B208" t="str">
-        <v>任天堂是世界的_____，索尼是宇宙的_____ !</v>
+        <v>学学比尔</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B209" t="str">
-        <v>全新抖音同款ins风潮流时尚生日礼物居家必备多功能万用懒人网红爆款特惠限量版_</v>
+        <v>批里批里淦杯</v>
       </c>
     </row>
     <row r="210">
@@ -2062,7 +2060,7 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B210" t="str">
-        <v>_也就图一乐，真想还得_</v>
+        <v>-天呐，比尔！你在干什么？你怎么能杀人！ -_     -你这比青蛙小便还下流的家伙，就由我的猎枪制裁。</v>
       </c>
     </row>
     <row r="211">
@@ -2070,31 +2068,31 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B211" t="str">
-        <v>金属</v>
+        <v>冬马小三</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B212" t="str">
-        <v>真鸡儿_</v>
+        <v>雪菜碧池</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B213" t="str">
-        <v>忘了他吧，我_养你</v>
+        <v>2333gkd那是真的批爆</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B214" t="str">
-        <v>vtuber</v>
+        <v>禁止在厕所_</v>
       </c>
     </row>
     <row r="215">
@@ -2102,7 +2100,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B215" t="str">
-        <v>阿苇</v>
+        <v>有基佬开我裤链</v>
       </c>
     </row>
     <row r="216">
@@ -2110,7 +2108,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B216" t="str">
-        <v>芦苇娘</v>
+        <v>咸豆腐脑天下第一</v>
       </c>
     </row>
     <row r="217">
@@ -2118,15 +2116,15 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B217" t="str">
-        <v>黄金回旋</v>
+        <v>甜豆腐脑天下第一</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B218" t="str">
-        <v>_3000</v>
+        <v>百事可乐</v>
       </c>
     </row>
     <row r="219">
@@ -2134,7 +2132,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B219" t="str">
-        <v>天堂制造</v>
+        <v>可口可乐</v>
       </c>
     </row>
     <row r="220">
@@ -2142,15 +2140,15 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B220" t="str">
-        <v>杀手皇后</v>
+        <v>牙签搅大缸</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B221" t="str">
-        <v>绯红之王</v>
+        <v>_超骚</v>
       </c>
     </row>
     <row r="222">
@@ -2158,7 +2156,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B222" t="str">
-        <v>砸瓦鲁多</v>
+        <v>用大蒜汁泡屌</v>
       </c>
     </row>
     <row r="223">
@@ -2166,7 +2164,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B223" t="str">
-        <v>疯狂钻石</v>
+        <v>辣椒酱抹菊花</v>
       </c>
     </row>
     <row r="224">
@@ -2174,7 +2172,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B224" t="str">
-        <v>白金之星</v>
+        <v>贫乳</v>
       </c>
     </row>
     <row r="225">
@@ -2182,39 +2180,39 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B225" t="str">
-        <v>黄金体验镇魂曲</v>
+        <v>巨乳</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B226" t="str">
-        <v>喇叭</v>
+        <v>_即是正义！</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B227" t="str">
-        <v>斯大林</v>
+        <v>这就是国家一级保护动物，_</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B228" t="str">
-        <v>刘姥姥</v>
+        <v>特朗普最新表态：_</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B229" t="str">
-        <v>吃华莱士</v>
+        <v>快手同款_，火热销售中！</v>
       </c>
     </row>
     <row r="230">
@@ -2222,7 +2220,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B230" t="str">
-        <v>喷射</v>
+        <v>黄脸婆</v>
       </c>
     </row>
     <row r="231">
@@ -2230,31 +2228,31 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B231" t="str">
-        <v>撸管</v>
+        <v>AC娘</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B232" t="str">
-        <v>看本子</v>
+        <v>我要成为新世界的_</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B233" t="str">
-        <v>NTR</v>
+        <v>-我喜欢用_做施法时的配菜。 -淦，老兄，你的性癖好jb怪啊！</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B234" t="str">
-        <v>射精管理</v>
+        <v>名侦探_</v>
       </c>
     </row>
     <row r="235">
@@ -2262,15 +2260,15 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B235" t="str">
-        <v>女装</v>
+        <v>路过的假面骑士</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B236" t="str">
-        <v>前列腺</v>
+        <v>请问您今天要来点_吗？</v>
       </c>
     </row>
     <row r="237">
@@ -2278,15 +2276,15 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B237" t="str">
-        <v>r20</v>
+        <v>狗比酱</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B238" t="str">
-        <v>_是_,而且是_的_你喜欢吗？</v>
+        <v>喵喵酱</v>
       </c>
     </row>
     <row r="239">
@@ -2294,7 +2292,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B239" t="str">
-        <v>马</v>
+        <v>阳光大姐</v>
       </c>
     </row>
     <row r="240">
@@ -2302,7 +2300,7 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B240" t="str">
-        <v>您的_没了</v>
+        <v>我_今天就是要一拳打爆你_的狗头</v>
       </c>
     </row>
     <row r="241">
@@ -2310,7 +2308,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B241" t="str">
-        <v>bog生来没有ma</v>
+        <v>穆斯林</v>
       </c>
     </row>
     <row r="242">
@@ -2318,7 +2316,7 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B242" t="str">
-        <v>天下漫友是一家,_</v>
+        <v>这里禁止养_</v>
       </c>
     </row>
     <row r="243">
@@ -2326,7 +2324,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B243" t="str">
-        <v>资本主义</v>
+        <v>抽烟喝酒烫头</v>
       </c>
     </row>
     <row r="244">
@@ -2334,7 +2332,7 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B244" t="str">
-        <v>_我草泥马</v>
+        <v>我最喜欢_</v>
       </c>
     </row>
     <row r="245">
@@ -2342,15 +2340,15 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B245" t="str">
-        <v>uk酱</v>
+        <v>人民广场1080度狂拽炫酷吊炸天大回旋空中手冲连续技</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B246" t="str">
-        <v>匿名版偶像</v>
+        <v>我最喜欢的食物是_</v>
       </c>
     </row>
     <row r="247">
@@ -2358,7 +2356,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B247" t="str">
-        <v>小碎骨</v>
+        <v>炸鸡，西瓜，葡萄汽水</v>
       </c>
     </row>
     <row r="248">
@@ -2366,7 +2364,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B248" t="str">
-        <v>飞蛾的排泄物</v>
+        <v>新鲜出炉的华莱士</v>
       </c>
     </row>
     <row r="249">
@@ -2374,7 +2372,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B249" t="str">
-        <v>一般通过肥肥</v>
+        <v>擦过精液的卫生纸</v>
       </c>
     </row>
     <row r="250">
@@ -2382,7 +2380,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B250" t="str">
-        <v>角虫</v>
+        <v>蟑螂</v>
       </c>
     </row>
     <row r="251">
@@ -2390,15 +2388,15 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B251" t="str">
-        <v>沙包</v>
+        <v>美洲大蠊</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B252" t="str">
-        <v>肥肥</v>
+        <v>随着“咔嚓”一声脆响，从蛋里钻出来一只_</v>
       </c>
     </row>
     <row r="253">
@@ -2406,7 +2404,7 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B253" t="str">
-        <v>丧尸</v>
+        <v>光头</v>
       </c>
     </row>
     <row r="254">
@@ -2414,31 +2412,31 @@
         <v>白色卡 - 回答卡</v>
       </c>
       <c r="B254" t="str">
-        <v>肥父</v>
+        <v>隔壁超市薯片半价</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B255" t="str">
-        <v>阴阳</v>
+        <v>无内鬼，来点_笑话</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B256" t="str">
-        <v>看小马</v>
+        <v>一开口就知道，老_了</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B257" t="str">
-        <v>撸管</v>
+        <v>人不能，至少不应该_</v>
       </c>
     </row>
     <row r="258">
@@ -2446,7 +2444,7 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B258" t="str">
-        <v>我一_发现_在_</v>
+        <v>警方在现场找到一具高度损坏的男性遗体，死因经检测为_</v>
       </c>
     </row>
     <row r="259">
@@ -2454,39 +2452,39 @@
         <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B259" t="str">
-        <v>只有_才能_</v>
+        <v>你们先走！我_</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B260" t="str">
-        <v>roll点</v>
+        <v>__虽好，但不要贪杯</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B261" t="str">
-        <v>岛摄</v>
+        <v>请勿将_放入_</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="str">
-        <v>白色卡 - 回答卡</v>
+        <v>黑色卡 - 提问卡</v>
       </c>
       <c r="B262" t="str">
-        <v>卡面来打</v>
+        <v>找_？就上阿里巴巴！</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="str">
-        <v>黑色卡 - 提问卡</v>
+        <v>白色卡 - 回答卡</v>
       </c>
       <c r="B263" t="str">
-        <v>如果在课堂上_的话学校生活就结束了</v>
+        <v>断罪小学</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[mod] update 2019-08-23 20:05
</commit_message>
<xml_diff>
--- a/CAH.xlsx
+++ b/CAH.xlsx
@@ -10,8 +10,21 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="3">
+  <numFmts count="16">
+    <numFmt numFmtId="5" formatCode="&quot;￥&quot;#,##0;&quot;￥&quot;\-#,##0"/>
+    <numFmt numFmtId="6" formatCode="&quot;￥&quot;#,##0;[Red]&quot;￥&quot;\-#,##0"/>
+    <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
+    <numFmt numFmtId="8" formatCode="&quot;￥&quot;#,##0.00;[Red]&quot;￥&quot;\-#,##0.00"/>
+    <numFmt numFmtId="23" formatCode="\$#,##0_);\(\$#,##0\)"/>
+    <numFmt numFmtId="24" formatCode="\$#,##0_);[Red]\(\$#,##0\)"/>
+    <numFmt numFmtId="25" formatCode="\$#,##0.00_);\(\$#,##0.00\)"/>
+    <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="390" formatCode="yyyy-MM-dd"/>
     <numFmt numFmtId="391" formatCode="yyyy-MM-dd\ HH:mm:ss"/>
   </numFmts>
@@ -378,7 +391,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="sheet1"/>
-  <dimension ref="A1:C263"/>
+  <dimension ref="A1:D263"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -390,6 +403,9 @@
       <c r="B1" t="str">
         <v>卡面内容</v>
       </c>
+      <c r="C1" t="str">
+        <v>标签</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -398,6 +414,9 @@
       <c r="B2" t="str">
         <v>如果在课堂上_的话学校生活就结束了</v>
       </c>
+      <c r="C2" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -406,6 +425,9 @@
       <c r="B3" t="str">
         <v>卡面来打</v>
       </c>
+      <c r="C3" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -414,6 +436,9 @@
       <c r="B4" t="str">
         <v>岛摄</v>
       </c>
+      <c r="C4" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -422,6 +447,9 @@
       <c r="B5" t="str">
         <v>roll点</v>
       </c>
+      <c r="C5" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -430,6 +458,9 @@
       <c r="B6" t="str">
         <v>只有_才能_</v>
       </c>
+      <c r="C6" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -438,6 +469,9 @@
       <c r="B7" t="str">
         <v>我一_发现_在_</v>
       </c>
+      <c r="C7" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -446,6 +480,9 @@
       <c r="B8" t="str">
         <v>撸管</v>
       </c>
+      <c r="C8" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -454,6 +491,9 @@
       <c r="B9" t="str">
         <v>看小马</v>
       </c>
+      <c r="C9" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -462,6 +502,9 @@
       <c r="B10" t="str">
         <v>阴阳</v>
       </c>
+      <c r="C10" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -470,6 +513,9 @@
       <c r="B11" t="str">
         <v>肥父</v>
       </c>
+      <c r="C11" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -478,6 +524,9 @@
       <c r="B12" t="str">
         <v>丧尸</v>
       </c>
+      <c r="C12" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -486,6 +535,9 @@
       <c r="B13" t="str">
         <v>肥肥</v>
       </c>
+      <c r="C13" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -494,6 +546,9 @@
       <c r="B14" t="str">
         <v>沙包</v>
       </c>
+      <c r="C14" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -502,6 +557,9 @@
       <c r="B15" t="str">
         <v>角虫</v>
       </c>
+      <c r="C15" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -510,6 +568,9 @@
       <c r="B16" t="str">
         <v>一般通过肥肥</v>
       </c>
+      <c r="C16" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -518,6 +579,9 @@
       <c r="B17" t="str">
         <v>飞蛾的排泄物</v>
       </c>
+      <c r="C17" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -526,6 +590,9 @@
       <c r="B18" t="str">
         <v>小碎骨</v>
       </c>
+      <c r="C18" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -534,6 +601,9 @@
       <c r="B19" t="str">
         <v>匿名版偶像</v>
       </c>
+      <c r="C19" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -542,6 +612,9 @@
       <c r="B20" t="str">
         <v>uk酱</v>
       </c>
+      <c r="C20" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
@@ -550,6 +623,9 @@
       <c r="B21" t="str">
         <v>_我草泥马</v>
       </c>
+      <c r="C21" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
@@ -558,6 +634,9 @@
       <c r="B22" t="str">
         <v>资本主义</v>
       </c>
+      <c r="C22" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
@@ -566,6 +645,9 @@
       <c r="B23" t="str">
         <v>天下漫友是一家,_</v>
       </c>
+      <c r="C23" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
@@ -574,6 +656,9 @@
       <c r="B24" t="str">
         <v>bog生来没有ma</v>
       </c>
+      <c r="C24" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
@@ -582,6 +667,9 @@
       <c r="B25" t="str">
         <v>您的_没了</v>
       </c>
+      <c r="C25" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
@@ -590,6 +678,9 @@
       <c r="B26" t="str">
         <v>马</v>
       </c>
+      <c r="C26" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
@@ -598,6 +689,9 @@
       <c r="B27" t="str">
         <v>_是_,而且是_的_你喜欢吗？</v>
       </c>
+      <c r="C27" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
@@ -606,6 +700,9 @@
       <c r="B28" t="str">
         <v>r20</v>
       </c>
+      <c r="C28" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
@@ -614,6 +711,9 @@
       <c r="B29" t="str">
         <v>前列腺</v>
       </c>
+      <c r="C29" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
@@ -622,6 +722,9 @@
       <c r="B30" t="str">
         <v>女装</v>
       </c>
+      <c r="C30" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
@@ -630,6 +733,9 @@
       <c r="B31" t="str">
         <v>射精管理</v>
       </c>
+      <c r="C31" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
@@ -638,6 +744,9 @@
       <c r="B32" t="str">
         <v>NTR</v>
       </c>
+      <c r="C32" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
@@ -646,6 +755,9 @@
       <c r="B33" t="str">
         <v>看本子</v>
       </c>
+      <c r="C33" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
@@ -654,6 +766,9 @@
       <c r="B34" t="str">
         <v>撸管</v>
       </c>
+      <c r="C34" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
@@ -662,6 +777,9 @@
       <c r="B35" t="str">
         <v>喷射</v>
       </c>
+      <c r="C35" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
@@ -670,6 +788,9 @@
       <c r="B36" t="str">
         <v>吃华莱士</v>
       </c>
+      <c r="C36" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
@@ -678,6 +799,9 @@
       <c r="B37" t="str">
         <v>刘姥姥</v>
       </c>
+      <c r="C37" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
@@ -686,6 +810,9 @@
       <c r="B38" t="str">
         <v>斯大林</v>
       </c>
+      <c r="C38" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
@@ -694,6 +821,9 @@
       <c r="B39" t="str">
         <v>喇叭</v>
       </c>
+      <c r="C39" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
@@ -702,6 +832,9 @@
       <c r="B40" t="str">
         <v>黄金体验镇魂曲</v>
       </c>
+      <c r="C40" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
@@ -710,6 +843,9 @@
       <c r="B41" t="str">
         <v>白金之星</v>
       </c>
+      <c r="C41" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
@@ -718,6 +854,9 @@
       <c r="B42" t="str">
         <v>疯狂钻石</v>
       </c>
+      <c r="C42" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
@@ -726,6 +865,9 @@
       <c r="B43" t="str">
         <v>砸瓦鲁多</v>
       </c>
+      <c r="C43" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
@@ -734,6 +876,9 @@
       <c r="B44" t="str">
         <v>绯红之王</v>
       </c>
+      <c r="C44" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
@@ -742,6 +887,9 @@
       <c r="B45" t="str">
         <v>杀手皇后</v>
       </c>
+      <c r="C45" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
@@ -750,6 +898,9 @@
       <c r="B46" t="str">
         <v>天堂制造</v>
       </c>
+      <c r="C46" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
@@ -758,6 +909,9 @@
       <c r="B47" t="str">
         <v>_3000</v>
       </c>
+      <c r="C47" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
@@ -766,6 +920,9 @@
       <c r="B48" t="str">
         <v>黄金回旋</v>
       </c>
+      <c r="C48" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
@@ -774,6 +931,9 @@
       <c r="B49" t="str">
         <v>芦苇娘</v>
       </c>
+      <c r="C49" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
@@ -782,6 +942,9 @@
       <c r="B50" t="str">
         <v>阿苇</v>
       </c>
+      <c r="C50" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
@@ -790,6 +953,9 @@
       <c r="B51" t="str">
         <v>vtuber</v>
       </c>
+      <c r="C51" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
@@ -798,6 +964,9 @@
       <c r="B52" t="str">
         <v>忘了他吧，我_养你</v>
       </c>
+      <c r="C52" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
@@ -806,6 +975,9 @@
       <c r="B53" t="str">
         <v>真鸡儿_</v>
       </c>
+      <c r="C53" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
@@ -814,6 +986,9 @@
       <c r="B54" t="str">
         <v>金属</v>
       </c>
+      <c r="C54" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
@@ -822,6 +997,9 @@
       <c r="B55" t="str">
         <v>_也就图一乐，真想还得_</v>
       </c>
+      <c r="C55" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
@@ -830,6 +1008,9 @@
       <c r="B56" t="str">
         <v>全新抖音同款ins风潮流时尚生日礼物居家必备多功能万用懒人网红爆款特惠限量版_</v>
       </c>
+      <c r="C56" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
@@ -838,6 +1019,9 @@
       <c r="B57" t="str">
         <v>任天堂是世界的_，索尼是宇宙的_!</v>
       </c>
+      <c r="C57" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
@@ -846,6 +1030,9 @@
       <c r="B58" t="str">
         <v>全世界的独立游戏制作人</v>
       </c>
+      <c r="C58" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
@@ -854,6 +1041,9 @@
       <c r="B59" t="str">
         <v>努力做到尿尿不分叉</v>
       </c>
+      <c r="C59" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
@@ -862,6 +1052,9 @@
       <c r="B60" t="str">
         <v>傻逼一号卢本伟准备就绪</v>
       </c>
+      <c r="C60" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
@@ -870,6 +1063,9 @@
       <c r="B61" t="str">
         <v>在bilibili突然发现了_</v>
       </c>
+      <c r="C61" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
@@ -878,6 +1074,9 @@
       <c r="B62" t="str">
         <v>手冲</v>
       </c>
+      <c r="C62" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
@@ -886,6 +1085,9 @@
       <c r="B63" t="str">
         <v>远在委内瑞拉的独立游戏制作人</v>
       </c>
+      <c r="C63" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
@@ -894,6 +1096,9 @@
       <c r="B64" t="str">
         <v>叙利亚打工仔</v>
       </c>
+      <c r="C64" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
@@ -902,6 +1107,9 @@
       <c r="B65" t="str">
         <v>new了一个对象</v>
       </c>
+      <c r="C65" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
@@ -910,6 +1118,9 @@
       <c r="B66" t="str">
         <v>尊敬的客户，您的_已到期，请及时充值</v>
       </c>
+      <c r="C66" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
@@ -918,6 +1129,9 @@
       <c r="B67" t="str">
         <v>寻找_特别行动小组，近日宣称_。</v>
       </c>
+      <c r="C67" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
@@ -926,6 +1140,9 @@
       <c r="B68" t="str">
         <v>胶佬</v>
       </c>
+      <c r="C68" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
@@ -934,6 +1151,9 @@
       <c r="B69" t="str">
         <v>手游玩家</v>
       </c>
+      <c r="C69" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
@@ -942,6 +1162,9 @@
       <c r="B70" t="str">
         <v>因为群员发布了_视频，群主被公开_。</v>
       </c>
+      <c r="C70" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
@@ -950,6 +1173,9 @@
       <c r="B71" t="str">
         <v>steam就是_启动器！</v>
       </c>
+      <c r="C71" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
@@ -958,6 +1184,9 @@
       <c r="B72" t="str">
         <v>恰柠檬</v>
       </c>
+      <c r="C72" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
@@ -966,6 +1195,9 @@
       <c r="B73" t="str">
         <v>反人类卡牌</v>
       </c>
+      <c r="C73" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
@@ -974,6 +1206,9 @@
       <c r="B74" t="str">
         <v>小黄油</v>
       </c>
+      <c r="C74" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
@@ -982,6 +1217,9 @@
       <c r="B75" t="str">
         <v>空气模拟器</v>
       </c>
+      <c r="C75" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
@@ -990,6 +1228,9 @@
       <c r="B76" t="str">
         <v>进入了坦克</v>
       </c>
+      <c r="C76" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
@@ -998,6 +1239,9 @@
       <c r="B77" t="str">
         <v>成为了微博红人榜最耀眼的星</v>
       </c>
+      <c r="C77" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
@@ -1006,6 +1250,9 @@
       <c r="B78" t="str">
         <v>单推孙笑川</v>
       </c>
+      <c r="C78" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
@@ -1014,6 +1261,9 @@
       <c r="B79" t="str">
         <v>暗杀刘波</v>
       </c>
+      <c r="C79" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
@@ -1022,6 +1272,9 @@
       <c r="B80" t="str">
         <v>我要成为_偶像，说罢裁判便抛下了妻女离去了。</v>
       </c>
+      <c r="C80" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
@@ -1030,6 +1283,9 @@
       <c r="B81" t="str">
         <v>听众朋友们欢迎收听深夜_广播节目，我是你们的好朋友_。</v>
       </c>
+      <c r="C81" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
@@ -1038,6 +1294,9 @@
       <c r="B82" t="str">
         <v>裁判</v>
       </c>
+      <c r="C82" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
@@ -1046,6 +1305,9 @@
       <c r="B83" t="str">
         <v>最后回答者</v>
       </c>
+      <c r="C83" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
@@ -1054,6 +1316,9 @@
       <c r="B84" t="str">
         <v>获胜者</v>
       </c>
+      <c r="C84" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
@@ -1062,6 +1327,9 @@
       <c r="B85" t="str">
         <v>打开了斗鱼7078973</v>
       </c>
+      <c r="C85" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
@@ -1070,6 +1338,9 @@
       <c r="B86" t="str">
         <v>用舌头走路</v>
       </c>
+      <c r="C86" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
@@ -1078,6 +1349,9 @@
       <c r="B87" t="str">
         <v>在抗日剧中参演日本天皇</v>
       </c>
+      <c r="C87" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
@@ -1086,6 +1360,9 @@
       <c r="B88" t="str">
         <v>乔碧萝殿下</v>
       </c>
+      <c r="C88" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
@@ -1094,6 +1371,9 @@
       <c r="B89" t="str">
         <v>郭德纲</v>
       </c>
+      <c r="C89" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="str">
@@ -1102,6 +1382,9 @@
       <c r="B90" t="str">
         <v>于谦</v>
       </c>
+      <c r="C90" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
@@ -1110,6 +1393,9 @@
       <c r="B91" t="str">
         <v>女装少年</v>
       </c>
+      <c r="C91" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
@@ -1118,6 +1404,9 @@
       <c r="B92" t="str">
         <v>大龄异装癖</v>
       </c>
+      <c r="C92" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="str">
@@ -1126,6 +1415,9 @@
       <c r="B93" t="str">
         <v>ATM</v>
       </c>
+      <c r="C93" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="str">
@@ -1134,6 +1426,9 @@
       <c r="B94" t="str">
         <v>为什么你会_！，难道你是_！？</v>
       </c>
+      <c r="C94" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="str">
@@ -1142,6 +1437,9 @@
       <c r="B95" t="str">
         <v>_一度成为2019年朝鲜最最流行。</v>
       </c>
+      <c r="C95" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="str">
@@ -1150,6 +1448,9 @@
       <c r="B96" t="str">
         <v>众所周知反人类卡牌除了白卡和黑卡，还有_卡。</v>
       </c>
+      <c r="C96" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="str">
@@ -1158,6 +1459,9 @@
       <c r="B97" t="str">
         <v>你妈升天</v>
       </c>
+      <c r="C97" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="str">
@@ -1166,6 +1470,9 @@
       <c r="B98" t="str">
         <v>大香肠</v>
       </c>
+      <c r="C98" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="str">
@@ -1174,6 +1481,9 @@
       <c r="B99" t="str">
         <v>_说：“是你守护了我吗？_”</v>
       </c>
+      <c r="C99" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="str">
@@ -1182,6 +1492,9 @@
       <c r="B100" t="str">
         <v>国产3A神作</v>
       </c>
+      <c r="C100" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="str">
@@ -1190,6 +1503,9 @@
       <c r="B101" t="str">
         <v>_爱上了_，在一个有星星的夜晚</v>
       </c>
+      <c r="C101" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="str">
@@ -1198,6 +1514,9 @@
       <c r="B102" t="str">
         <v>经证实，被_撞飞至40米高空的_，被判为碰瓷行为，现已依法入狱。</v>
       </c>
+      <c r="C102" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="str">
@@ -1206,6 +1525,9 @@
       <c r="B103" t="str">
         <v>为了攻打养老院我们派出了，20多名英勇的_。</v>
       </c>
+      <c r="C103" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="str">
@@ -1214,6 +1536,9 @@
       <c r="B104" t="str">
         <v>《恋上妹妹的_》一经发售便风靡全球</v>
       </c>
+      <c r="C104" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="str">
@@ -1222,6 +1547,9 @@
       <c r="B105" t="str">
         <v>公司新增一个_岗位，月薪近20W。</v>
       </c>
+      <c r="C105" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="str">
@@ -1230,6 +1558,9 @@
       <c r="B106" t="str">
         <v>逼乎大神</v>
       </c>
+      <c r="C106" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="str">
@@ -1238,6 +1569,9 @@
       <c r="B107" t="str">
         <v>啊</v>
       </c>
+      <c r="C107" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="str">
@@ -1246,6 +1580,9 @@
       <c r="B108" t="str">
         <v>看_也就图一乐，真要_还得看_</v>
       </c>
+      <c r="C108" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="str">
@@ -1254,6 +1591,9 @@
       <c r="B109" t="str">
         <v>看到这个我气得浑身发抖， 大热天的全身冷汗，手脚冰凉， 这个社会还能不能好了， 到底要怎么样你们才满意 眼泪不争气的流了下来 ，_上到处充斥着对 _的压迫， 他们何时才能真正的站起来？</v>
       </c>
+      <c r="C109" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="str">
@@ -1262,6 +1602,9 @@
       <c r="B110" t="str">
         <v>无内鬼，发点_</v>
       </c>
+      <c r="C110" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="str">
@@ -1270,6 +1613,9 @@
       <c r="B111" t="str">
         <v>重生之我是_</v>
       </c>
+      <c r="C111" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="str">
@@ -1278,6 +1624,9 @@
       <c r="B112" t="str">
         <v>我_ ，在那儿他们都叫我_ ！</v>
       </c>
+      <c r="C112" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="str">
@@ -1286,6 +1635,9 @@
       <c r="B113" t="str">
         <v>说起来很下流，我看见_boki了</v>
       </c>
+      <c r="C113" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="str">
@@ -1294,6 +1646,9 @@
       <c r="B114" t="str">
         <v>我支持_ ！你们可以打我了！</v>
       </c>
+      <c r="C114" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="str">
@@ -1302,6 +1657,9 @@
       <c r="B115" t="str">
         <v>_，FBI Open up！</v>
       </c>
+      <c r="C115" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="str">
@@ -1310,6 +1668,9 @@
       <c r="B116" t="str">
         <v>人不能_，至少不该</v>
       </c>
+      <c r="C116" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="str">
@@ -1318,6 +1679,9 @@
       <c r="B117" t="str">
         <v>天哪！这是什么神仙_鸭！！我坐地排卵！</v>
       </c>
+      <c r="C117" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="str">
@@ -1326,6 +1690,9 @@
       <c r="B118" t="str">
         <v>在_有一个永恒话题，那就是_</v>
       </c>
+      <c r="C118" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="str">
@@ -1334,6 +1701,9 @@
       <c r="B119" t="str">
         <v>《如果早知道_也会被性侵》</v>
       </c>
+      <c r="C119" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="str">
@@ -1342,6 +1712,9 @@
       <c r="B120" t="str">
         <v>都9012年了，你还在_？</v>
       </c>
+      <c r="C120" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="str">
@@ -1350,6 +1723,9 @@
       <c r="B121" t="str">
         <v>_2077</v>
       </c>
+      <c r="C121" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="str">
@@ -1358,6 +1734,9 @@
       <c r="B122" t="str">
         <v>海绵宝宝</v>
       </c>
+      <c r="C122" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="str">
@@ -1366,6 +1745,9 @@
       <c r="B123" t="str">
         <v>感染菜花</v>
       </c>
+      <c r="C123" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="str">
@@ -1374,6 +1756,9 @@
       <c r="B124" t="str">
         <v>出卖斯大林</v>
       </c>
+      <c r="C124" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="str">
@@ -1382,6 +1767,9 @@
       <c r="B125" t="str">
         <v>跑团</v>
       </c>
+      <c r="C125" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="str">
@@ -1390,6 +1778,9 @@
       <c r="B126" t="str">
         <v>魔法少女</v>
       </c>
+      <c r="C126" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="str">
@@ -1398,6 +1789,9 @@
       <c r="B127" t="str">
         <v>键盘侠</v>
       </c>
+      <c r="C127" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="str">
@@ -1406,6 +1800,9 @@
       <c r="B128" t="str">
         <v>野兽先辈</v>
       </c>
+      <c r="C128" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="str">
@@ -1414,6 +1811,9 @@
       <c r="B129" t="str">
         <v>倒悬打飞机</v>
       </c>
+      <c r="C129" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="str">
@@ -1422,6 +1822,9 @@
       <c r="B130" t="str">
         <v>那么答案只有一个了！_ _</v>
       </c>
+      <c r="C130" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="str">
@@ -1430,6 +1833,9 @@
       <c r="B131" t="str">
         <v>向你宣誓效忠</v>
       </c>
+      <c r="C131" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="str">
@@ -1438,6 +1844,9 @@
       <c r="B132" t="str">
         <v>洛阳亲友如相问，_ _</v>
       </c>
+      <c r="C132" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="str">
@@ -1446,6 +1855,9 @@
       <c r="B133" t="str">
         <v>鲨鱼抱枕</v>
       </c>
+      <c r="C133" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="str">
@@ -1454,6 +1866,9 @@
       <c r="B134" t="str">
         <v>飞天大草</v>
       </c>
+      <c r="C134" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="str">
@@ -1462,6 +1877,9 @@
       <c r="B135" t="str">
         <v>百般武艺，此乃_</v>
       </c>
+      <c r="C135" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="str">
@@ -1470,6 +1888,9 @@
       <c r="B136" t="str">
         <v>没有_便无法_了吗？，_岂是如此不便之物！</v>
       </c>
+      <c r="C136" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="str">
@@ -1478,6 +1899,9 @@
       <c r="B137" t="str">
         <v>陈睿</v>
       </c>
+      <c r="C137" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="str">
@@ -1486,6 +1910,9 @@
       <c r="B138" t="str">
         <v>徐逸</v>
       </c>
+      <c r="C138" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="str">
@@ -1494,6 +1921,9 @@
       <c r="B139" t="str">
         <v>塞进菊花</v>
       </c>
+      <c r="C139" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="str">
@@ -1502,6 +1932,9 @@
       <c r="B140" t="str">
         <v>你妈炸了</v>
       </c>
+      <c r="C140" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="str">
@@ -1510,6 +1943,9 @@
       <c r="B141" t="str">
         <v>机械烈海王</v>
       </c>
+      <c r="C141" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="str">
@@ -1518,6 +1954,9 @@
       <c r="B142" t="str">
         <v>人群中钻出来一个_</v>
       </c>
+      <c r="C142" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="str">
@@ -1526,6 +1965,9 @@
       <c r="B143" t="str">
         <v>草莓糖浆</v>
       </c>
+      <c r="C143" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="str">
@@ -1534,6 +1976,9 @@
       <c r="B144" t="str">
         <v>草莓幼女</v>
       </c>
+      <c r="C144" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="str">
@@ -1542,6 +1987,9 @@
       <c r="B145" t="str">
         <v>三个月没洗的</v>
       </c>
+      <c r="C145" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="str">
@@ -1550,6 +1998,9 @@
       <c r="B146" t="str">
         <v>施主</v>
       </c>
+      <c r="C146" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="str">
@@ -1558,6 +2009,9 @@
       <c r="B147" t="str">
         <v>自私的神</v>
       </c>
+      <c r="C147" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="str">
@@ -1566,6 +2020,9 @@
       <c r="B148" t="str">
         <v>jojo</v>
       </c>
+      <c r="C148" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="str">
@@ -1574,6 +2031,9 @@
       <c r="B149" t="str">
         <v>-施主，这是什么漫画？ -是_</v>
       </c>
+      <c r="C149" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="str">
@@ -1582,6 +2042,9 @@
       <c r="B150" t="str">
         <v>滚铁环</v>
       </c>
+      <c r="C150" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="str">
@@ -1590,6 +2053,9 @@
       <c r="B151" t="str">
         <v>欧吉车技腐乳句句然到雾入饭卡死了</v>
       </c>
+      <c r="C151" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="str">
@@ -1598,6 +2064,9 @@
       <c r="B152" t="str">
         <v>欧拉欧拉欧拉</v>
       </c>
+      <c r="C152" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="str">
@@ -1606,6 +2075,9 @@
       <c r="B153" t="str">
         <v>-我就是憨批之王   -__    -你赢了</v>
       </c>
+      <c r="C153" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="str">
@@ -1614,6 +2086,9 @@
       <c r="B154" t="str">
         <v>这是是什么神仙_啊！</v>
       </c>
+      <c r="C154" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="str">
@@ -1622,6 +2097,9 @@
       <c r="B155" t="str">
         <v>宝藏男孩</v>
       </c>
+      <c r="C155" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="str">
@@ -1630,6 +2108,9 @@
       <c r="B156" t="str">
         <v>这个版本我们决定削弱_，增强_</v>
       </c>
+      <c r="C156" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="str">
@@ -1638,6 +2119,9 @@
       <c r="B157" t="str">
         <v>你们没有_吗？</v>
       </c>
+      <c r="C157" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="str">
@@ -1646,6 +2130,9 @@
       <c r="B158" t="str">
         <v>-今天岛上没有智障 -淦！是_！</v>
       </c>
+      <c r="C158" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="str">
@@ -1654,6 +2141,9 @@
       <c r="B159" t="str">
         <v>微积分</v>
       </c>
+      <c r="C159" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="str">
@@ -1662,6 +2152,9 @@
       <c r="B160" t="str">
         <v>N98</v>
       </c>
+      <c r="C160" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="str">
@@ -1670,6 +2163,9 @@
       <c r="B161" t="str">
         <v>台妹</v>
       </c>
+      <c r="C161" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="str">
@@ -1678,6 +2174,9 @@
       <c r="B162" t="str">
         <v>发色图</v>
       </c>
+      <c r="C162" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="str">
@@ -1686,6 +2185,9 @@
       <c r="B163" t="str">
         <v>狂拽炫酷吊炸天</v>
       </c>
+      <c r="C163" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="str">
@@ -1694,6 +2196,9 @@
       <c r="B164" t="str">
         <v>活塞运动</v>
       </c>
+      <c r="C164" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="str">
@@ -1702,6 +2207,9 @@
       <c r="B165" t="str">
         <v>上上下下左左右右BABA</v>
       </c>
+      <c r="C165" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="str">
@@ -1710,6 +2218,9 @@
       <c r="B166" t="str">
         <v>妹妹的内裤</v>
       </c>
+      <c r="C166" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="str">
@@ -1718,6 +2229,9 @@
       <c r="B167" t="str">
         <v>我们可以看到，监控画面中的这位男子正在_</v>
       </c>
+      <c r="C167" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="str">
@@ -1726,6 +2240,9 @@
       <c r="B168" t="str">
         <v>做超屌的720度大回旋</v>
       </c>
+      <c r="C168" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="str">
@@ -1734,6 +2251,9 @@
       <c r="B169" t="str">
         <v>真tm牛逼，搞得我想一拳打进_的_里。</v>
       </c>
+      <c r="C169" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="str">
@@ -1742,6 +2262,9 @@
       <c r="B170" t="str">
         <v>里神乐</v>
       </c>
+      <c r="C170" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="str">
@@ -1750,6 +2273,9 @@
       <c r="B171" t="str">
         <v>恨不得把蛋都塞进_里</v>
       </c>
+      <c r="C171" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="str">
@@ -1758,6 +2284,9 @@
       <c r="B172" t="str">
         <v>马眼</v>
       </c>
+      <c r="C172" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="str">
@@ -1766,6 +2295,9 @@
       <c r="B173" t="str">
         <v>切尔诺贝利</v>
       </c>
+      <c r="C173" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="str">
@@ -1774,6 +2306,9 @@
       <c r="B174" t="str">
         <v>这就是_吗？</v>
       </c>
+      <c r="C174" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="str">
@@ -1782,6 +2317,9 @@
       <c r="B175" t="str">
         <v>哇(=ﾟωﾟ)=</v>
       </c>
+      <c r="C175" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="str">
@@ -1790,6 +2328,9 @@
       <c r="B176" t="str">
         <v>城墙</v>
       </c>
+      <c r="C176" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="str">
@@ -1798,6 +2339,9 @@
       <c r="B177" t="str">
         <v>(ノﾟ∀ﾟ)ノ举高高</v>
       </c>
+      <c r="C177" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="str">
@@ -1806,6 +2350,9 @@
       <c r="B178" t="str">
         <v>(　^ω^)</v>
       </c>
+      <c r="C178" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="str">
@@ -1814,6 +2361,9 @@
       <c r="B179" t="str">
         <v>尼哥</v>
       </c>
+      <c r="C179" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="str">
@@ -1822,6 +2372,9 @@
       <c r="B180" t="str">
         <v>furry</v>
       </c>
+      <c r="C180" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="str">
@@ -1830,6 +2383,9 @@
       <c r="B181" t="str">
         <v>兽耳娘</v>
       </c>
+      <c r="C181" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="str">
@@ -1838,6 +2394,9 @@
       <c r="B182" t="str">
         <v>你被捕了，因为你_</v>
       </c>
+      <c r="C182" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="str">
@@ -1846,6 +2405,9 @@
       <c r="B183" t="str">
         <v>用套套吹气球</v>
       </c>
+      <c r="C183" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="str">
@@ -1854,6 +2416,9 @@
       <c r="B184" t="str">
         <v>在厕所日马桶排水口</v>
       </c>
+      <c r="C184" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="str">
@@ -1862,6 +2427,9 @@
       <c r="B185" t="str">
         <v>幼女</v>
       </c>
+      <c r="C185" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="str">
@@ -1870,6 +2438,9 @@
       <c r="B186" t="str">
         <v>幼男</v>
       </c>
+      <c r="C186" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="str">
@@ -1878,6 +2449,9 @@
       <c r="B187" t="str">
         <v>看幼女视频</v>
       </c>
+      <c r="C187" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="str">
@@ -1886,6 +2460,9 @@
       <c r="B188" t="str">
         <v>_批发，量大从优</v>
       </c>
+      <c r="C188" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="str">
@@ -1894,6 +2471,9 @@
       <c r="B189" t="str">
         <v>你爸的跳蛋漏电了</v>
       </c>
+      <c r="C189" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="str">
@@ -1902,6 +2482,9 @@
       <c r="B190" t="str">
         <v>青梅竹马</v>
       </c>
+      <c r="C190" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="str">
@@ -1910,6 +2493,9 @@
       <c r="B191" t="str">
         <v>穿着女装的你爸</v>
       </c>
+      <c r="C191" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="str">
@@ -1918,6 +2504,9 @@
       <c r="B192" t="str">
         <v>你在嫖娼时发现，这里的头牌居然是_</v>
       </c>
+      <c r="C192" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="str">
@@ -1926,6 +2515,9 @@
       <c r="B193" t="str">
         <v>《_名言选》是今年的畅销书</v>
       </c>
+      <c r="C193" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="str">
@@ -1934,6 +2526,9 @@
       <c r="B194" t="str">
         <v>五分钟带你看完_</v>
       </c>
+      <c r="C194" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="str">
@@ -1942,6 +2537,9 @@
       <c r="B195" t="str">
         <v>只有我一个人_吗？</v>
       </c>
+      <c r="C195" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="str">
@@ -1950,6 +2548,9 @@
       <c r="B196" t="str">
         <v>在变身魔法少女之后裸奔，结果被城管抓走</v>
       </c>
+      <c r="C196" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="str">
@@ -1958,6 +2559,9 @@
       <c r="B197" t="str">
         <v>他居然使用_挡下了所有的攻击！</v>
       </c>
+      <c r="C197" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="str">
@@ -1966,6 +2570,9 @@
       <c r="B198" t="str">
         <v>_现已加入肯德基豪华午餐</v>
       </c>
+      <c r="C198" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="str">
@@ -1974,6 +2581,9 @@
       <c r="B199" t="str">
         <v>_，你一定不懂吧。</v>
       </c>
+      <c r="C199" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="str">
@@ -1982,6 +2592,9 @@
       <c r="B200" t="str">
         <v>空中转体两周半</v>
       </c>
+      <c r="C200" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="str">
@@ -1990,6 +2603,9 @@
       <c r="B201" t="str">
         <v>没有什么比爱情的力量更强大，除了_</v>
       </c>
+      <c r="C201" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="str">
@@ -1998,6 +2614,9 @@
       <c r="B202" t="str">
         <v>人_，就会死。</v>
       </c>
+      <c r="C202" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="str">
@@ -2006,6 +2625,9 @@
       <c r="B203" t="str">
         <v>被杀</v>
       </c>
+      <c r="C203" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="str">
@@ -2014,6 +2636,9 @@
       <c r="B204" t="str">
         <v>这是失传已久的_神功！你到底是谁！</v>
       </c>
+      <c r="C204" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="str">
@@ -2022,6 +2647,9 @@
       <c r="B205" t="str">
         <v>以前我没得选择，现在我想做个_</v>
       </c>
+      <c r="C205" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="str">
@@ -2030,6 +2658,9 @@
       <c r="B206" t="str">
         <v>对不起，我是_</v>
       </c>
+      <c r="C206" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="str">
@@ -2038,6 +2669,9 @@
       <c r="B207" t="str">
         <v>_才有怜悯之心，我没有</v>
       </c>
+      <c r="C207" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="str">
@@ -2046,6 +2680,9 @@
       <c r="B208" t="str">
         <v>学学比尔</v>
       </c>
+      <c r="C208" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="str">
@@ -2054,6 +2691,9 @@
       <c r="B209" t="str">
         <v>批里批里淦杯</v>
       </c>
+      <c r="C209" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="str">
@@ -2062,6 +2702,9 @@
       <c r="B210" t="str">
         <v>-天呐，比尔！你在干什么？你怎么能杀人！ -_     -你这比青蛙小便还下流的家伙，就由我的猎枪制裁。</v>
       </c>
+      <c r="C210" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="str">
@@ -2070,6 +2713,9 @@
       <c r="B211" t="str">
         <v>冬马小三</v>
       </c>
+      <c r="C211" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="str">
@@ -2078,6 +2724,9 @@
       <c r="B212" t="str">
         <v>雪菜碧池</v>
       </c>
+      <c r="C212" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="str">
@@ -2086,6 +2735,9 @@
       <c r="B213" t="str">
         <v>2333gkd那是真的批爆</v>
       </c>
+      <c r="C213" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="str">
@@ -2094,6 +2746,9 @@
       <c r="B214" t="str">
         <v>禁止在厕所_</v>
       </c>
+      <c r="C214" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="str">
@@ -2102,6 +2757,9 @@
       <c r="B215" t="str">
         <v>有基佬开我裤链</v>
       </c>
+      <c r="C215" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="str">
@@ -2110,6 +2768,9 @@
       <c r="B216" t="str">
         <v>咸豆腐脑天下第一</v>
       </c>
+      <c r="C216" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="str">
@@ -2118,6 +2779,9 @@
       <c r="B217" t="str">
         <v>甜豆腐脑天下第一</v>
       </c>
+      <c r="C217" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="str">
@@ -2126,6 +2790,9 @@
       <c r="B218" t="str">
         <v>百事可乐</v>
       </c>
+      <c r="C218" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="str">
@@ -2134,6 +2801,9 @@
       <c r="B219" t="str">
         <v>可口可乐</v>
       </c>
+      <c r="C219" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" t="str">
@@ -2142,6 +2812,9 @@
       <c r="B220" t="str">
         <v>牙签搅大缸</v>
       </c>
+      <c r="C220" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="str">
@@ -2150,6 +2823,9 @@
       <c r="B221" t="str">
         <v>_超骚</v>
       </c>
+      <c r="C221" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222" t="str">
@@ -2158,6 +2834,9 @@
       <c r="B222" t="str">
         <v>用大蒜汁泡屌</v>
       </c>
+      <c r="C222" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="223">
       <c r="A223" t="str">
@@ -2166,6 +2845,9 @@
       <c r="B223" t="str">
         <v>辣椒酱抹菊花</v>
       </c>
+      <c r="C223" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="224">
       <c r="A224" t="str">
@@ -2174,6 +2856,9 @@
       <c r="B224" t="str">
         <v>贫乳</v>
       </c>
+      <c r="C224" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="225">
       <c r="A225" t="str">
@@ -2182,6 +2867,9 @@
       <c r="B225" t="str">
         <v>巨乳</v>
       </c>
+      <c r="C225" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="226">
       <c r="A226" t="str">
@@ -2190,6 +2878,9 @@
       <c r="B226" t="str">
         <v>_即是正义！</v>
       </c>
+      <c r="C226" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="str">
@@ -2198,6 +2889,9 @@
       <c r="B227" t="str">
         <v>这就是国家一级保护动物，_</v>
       </c>
+      <c r="C227" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="228">
       <c r="A228" t="str">
@@ -2206,6 +2900,9 @@
       <c r="B228" t="str">
         <v>特朗普最新表态：_</v>
       </c>
+      <c r="C228" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="str">
@@ -2214,6 +2911,9 @@
       <c r="B229" t="str">
         <v>快手同款_，火热销售中！</v>
       </c>
+      <c r="C229" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230" t="str">
@@ -2222,6 +2922,9 @@
       <c r="B230" t="str">
         <v>黄脸婆</v>
       </c>
+      <c r="C230" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="231">
       <c r="A231" t="str">
@@ -2230,6 +2933,9 @@
       <c r="B231" t="str">
         <v>AC娘</v>
       </c>
+      <c r="C231" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="232">
       <c r="A232" t="str">
@@ -2238,6 +2944,9 @@
       <c r="B232" t="str">
         <v>我要成为新世界的_</v>
       </c>
+      <c r="C232" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" t="str">
@@ -2246,6 +2955,9 @@
       <c r="B233" t="str">
         <v>-我喜欢用_做施法时的配菜。 -淦，老兄，你的性癖好jb怪啊！</v>
       </c>
+      <c r="C233" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="str">
@@ -2254,6 +2966,9 @@
       <c r="B234" t="str">
         <v>名侦探_</v>
       </c>
+      <c r="C234" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="235">
       <c r="A235" t="str">
@@ -2262,6 +2977,9 @@
       <c r="B235" t="str">
         <v>路过的假面骑士</v>
       </c>
+      <c r="C235" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="str">
@@ -2270,6 +2988,9 @@
       <c r="B236" t="str">
         <v>请问您今天要来点_吗？</v>
       </c>
+      <c r="C236" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237" t="str">
@@ -2278,6 +2999,9 @@
       <c r="B237" t="str">
         <v>狗比酱</v>
       </c>
+      <c r="C237" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="str">
@@ -2286,6 +3010,9 @@
       <c r="B238" t="str">
         <v>喵喵酱</v>
       </c>
+      <c r="C238" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239" t="str">
@@ -2294,6 +3021,9 @@
       <c r="B239" t="str">
         <v>阳光大姐</v>
       </c>
+      <c r="C239" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="str">
@@ -2302,6 +3032,9 @@
       <c r="B240" t="str">
         <v>我_今天就是要一拳打爆你_的狗头</v>
       </c>
+      <c r="C240" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="str">
@@ -2310,6 +3043,9 @@
       <c r="B241" t="str">
         <v>穆斯林</v>
       </c>
+      <c r="C241" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="str">
@@ -2318,6 +3054,9 @@
       <c r="B242" t="str">
         <v>这里禁止养_</v>
       </c>
+      <c r="C242" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243" t="str">
@@ -2326,6 +3065,9 @@
       <c r="B243" t="str">
         <v>抽烟喝酒烫头</v>
       </c>
+      <c r="C243" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="str">
@@ -2334,6 +3076,9 @@
       <c r="B244" t="str">
         <v>我最喜欢_</v>
       </c>
+      <c r="C244" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="str">
@@ -2342,6 +3087,9 @@
       <c r="B245" t="str">
         <v>人民广场1080度狂拽炫酷吊炸天大回旋空中手冲连续技</v>
       </c>
+      <c r="C245" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246" t="str">
@@ -2350,6 +3098,9 @@
       <c r="B246" t="str">
         <v>我最喜欢的食物是_</v>
       </c>
+      <c r="C246" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="247">
       <c r="A247" t="str">
@@ -2358,6 +3109,9 @@
       <c r="B247" t="str">
         <v>炸鸡，西瓜，葡萄汽水</v>
       </c>
+      <c r="C247" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248" t="str">
@@ -2366,6 +3120,9 @@
       <c r="B248" t="str">
         <v>新鲜出炉的华莱士</v>
       </c>
+      <c r="C248" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="249">
       <c r="A249" t="str">
@@ -2374,6 +3131,9 @@
       <c r="B249" t="str">
         <v>擦过精液的卫生纸</v>
       </c>
+      <c r="C249" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="250">
       <c r="A250" t="str">
@@ -2382,6 +3142,9 @@
       <c r="B250" t="str">
         <v>蟑螂</v>
       </c>
+      <c r="C250" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="251">
       <c r="A251" t="str">
@@ -2390,6 +3153,9 @@
       <c r="B251" t="str">
         <v>美洲大蠊</v>
       </c>
+      <c r="C251" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252" t="str">
@@ -2398,6 +3164,9 @@
       <c r="B252" t="str">
         <v>随着“咔嚓”一声脆响，从蛋里钻出来一只_</v>
       </c>
+      <c r="C252" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="253">
       <c r="A253" t="str">
@@ -2406,6 +3175,9 @@
       <c r="B253" t="str">
         <v>光头</v>
       </c>
+      <c r="C253" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="254">
       <c r="A254" t="str">
@@ -2414,6 +3186,9 @@
       <c r="B254" t="str">
         <v>隔壁超市薯片半价</v>
       </c>
+      <c r="C254" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="255">
       <c r="A255" t="str">
@@ -2422,6 +3197,9 @@
       <c r="B255" t="str">
         <v>无内鬼，来点_笑话</v>
       </c>
+      <c r="C255" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="256">
       <c r="A256" t="str">
@@ -2430,6 +3208,9 @@
       <c r="B256" t="str">
         <v>一开口就知道，老_了</v>
       </c>
+      <c r="C256" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="257">
       <c r="A257" t="str">
@@ -2438,6 +3219,9 @@
       <c r="B257" t="str">
         <v>人不能，至少不应该_</v>
       </c>
+      <c r="C257" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="258">
       <c r="A258" t="str">
@@ -2446,6 +3230,9 @@
       <c r="B258" t="str">
         <v>警方在现场找到一具高度损坏的男性遗体，死因经检测为_</v>
       </c>
+      <c r="C258" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="259">
       <c r="A259" t="str">
@@ -2454,6 +3241,9 @@
       <c r="B259" t="str">
         <v>你们先走！我_</v>
       </c>
+      <c r="C259" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="260">
       <c r="A260" t="str">
@@ -2462,6 +3252,9 @@
       <c r="B260" t="str">
         <v>__虽好，但不要贪杯</v>
       </c>
+      <c r="C260" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="261">
       <c r="A261" t="str">
@@ -2470,6 +3263,9 @@
       <c r="B261" t="str">
         <v>请勿将_放入_</v>
       </c>
+      <c r="C261" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="262">
       <c r="A262" t="str">
@@ -2478,6 +3274,9 @@
       <c r="B262" t="str">
         <v>找_？就上阿里巴巴！</v>
       </c>
+      <c r="C262" t="str">
+        <v>["玩家自制"]</v>
+      </c>
     </row>
     <row r="263">
       <c r="A263" t="str">
@@ -2485,6 +3284,9 @@
       </c>
       <c r="B263" t="str">
         <v>断罪小学</v>
+      </c>
+      <c r="C263" t="str">
+        <v>["玩家自制"]</v>
       </c>
     </row>
   </sheetData>

</xml_diff>